<commit_message>
Added Cluster 2 Results
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ali/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ali/Documents/CST4599 Thesis/CST4599/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7ED18E-33B4-1B4C-B6D7-323928402A27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374CF6A8-DF8C-A24B-9388-B73327934777}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 Active Worker" sheetId="1" r:id="rId1"/>
@@ -269,6 +269,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
@@ -281,14 +287,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -299,14 +299,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7279,16 +7279,13 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -8240,16 +8237,13 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -16242,7 +16236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView topLeftCell="E13" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <selection activeCell="O1" sqref="O1:S1"/>
     </sheetView>
   </sheetViews>
@@ -16265,32 +16259,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="61" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="O1" s="21" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="O1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
     </row>
     <row r="2" spans="1:19" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
     </row>
     <row r="3" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -16321,7 +16315,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -16334,7 +16328,7 @@
         <v>0.39700000000000002</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="P4" s="4" t="s">
@@ -16351,7 +16345,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -16362,7 +16356,7 @@
         <v>0.09</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="O5" s="11"/>
+      <c r="O5" s="13"/>
       <c r="P5" s="4" t="s">
         <v>6</v>
       </c>
@@ -16377,7 +16371,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -16388,7 +16382,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="O6" s="11"/>
+      <c r="O6" s="13"/>
       <c r="P6" s="4" t="s">
         <v>7</v>
       </c>
@@ -16403,7 +16397,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -16414,7 +16408,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="O7" s="11"/>
+      <c r="O7" s="13"/>
       <c r="P7" s="5" t="s">
         <v>8</v>
       </c>
@@ -16429,7 +16423,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -16442,7 +16436,7 @@
         <v>5.4930000000000003</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="O8" s="10" t="s">
+      <c r="O8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="P8" s="6" t="s">
@@ -16459,7 +16453,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -16470,7 +16464,7 @@
         <v>15.504</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="O9" s="10"/>
+      <c r="O9" s="12"/>
       <c r="P9" s="6" t="s">
         <v>6</v>
       </c>
@@ -16485,7 +16479,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
@@ -16496,7 +16490,7 @@
         <v>28.515000000000001</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="O10" s="10"/>
+      <c r="O10" s="12"/>
       <c r="P10" s="6" t="s">
         <v>7</v>
       </c>
@@ -16511,7 +16505,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
@@ -16522,7 +16516,7 @@
         <v>41.524000000000001</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="O11" s="10"/>
+      <c r="O11" s="12"/>
       <c r="P11" s="7" t="s">
         <v>8</v>
       </c>
@@ -16537,7 +16531,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -16550,7 +16544,7 @@
         <v>2.4830000000000001</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="O12" s="11" t="s">
+      <c r="O12" s="13" t="s">
         <v>10</v>
       </c>
       <c r="P12" s="4" t="s">
@@ -16567,7 +16561,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -16578,7 +16572,7 @@
         <v>3.4790000000000001</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="O13" s="11"/>
+      <c r="O13" s="13"/>
       <c r="P13" s="4" t="s">
         <v>6</v>
       </c>
@@ -16593,7 +16587,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
@@ -16604,7 +16598,7 @@
         <v>4.4829999999999997</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="O14" s="11"/>
+      <c r="O14" s="13"/>
       <c r="P14" s="4" t="s">
         <v>7</v>
       </c>
@@ -16619,7 +16613,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
@@ -16630,7 +16624,7 @@
         <v>6.4829999999999997</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="O15" s="11"/>
+      <c r="O15" s="13"/>
       <c r="P15" s="5" t="s">
         <v>8</v>
       </c>
@@ -16645,7 +16639,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -16658,7 +16652,7 @@
         <v>2.4769999999999999</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="O16" s="10" t="s">
+      <c r="O16" s="12" t="s">
         <v>11</v>
       </c>
       <c r="P16" s="6" t="s">
@@ -16675,7 +16669,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
@@ -16686,7 +16680,7 @@
         <v>5.4820000000000002</v>
       </c>
       <c r="E17" s="6"/>
-      <c r="O17" s="10"/>
+      <c r="O17" s="12"/>
       <c r="P17" s="6" t="s">
         <v>6</v>
       </c>
@@ -16701,7 +16695,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="6" t="s">
         <v>7</v>
       </c>
@@ -16712,7 +16706,7 @@
         <v>9.5</v>
       </c>
       <c r="E18" s="6"/>
-      <c r="O18" s="10"/>
+      <c r="O18" s="12"/>
       <c r="P18" s="6" t="s">
         <v>7</v>
       </c>
@@ -16727,7 +16721,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="7" t="s">
         <v>8</v>
       </c>
@@ -16738,7 +16732,7 @@
         <v>13.497</v>
       </c>
       <c r="E19" s="6"/>
-      <c r="O19" s="10"/>
+      <c r="O19" s="12"/>
       <c r="P19" s="7" t="s">
         <v>8</v>
       </c>
@@ -16753,7 +16747,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -16766,7 +16760,7 @@
         <v>44.503999999999998</v>
       </c>
       <c r="E20" s="4"/>
-      <c r="O20" s="11" t="s">
+      <c r="O20" s="13" t="s">
         <v>12</v>
       </c>
       <c r="P20" s="4" t="s">
@@ -16783,7 +16777,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
@@ -16794,7 +16788,7 @@
         <v>181.61799999999999</v>
       </c>
       <c r="E21" s="4"/>
-      <c r="O21" s="11"/>
+      <c r="O21" s="13"/>
       <c r="P21" s="4" t="s">
         <v>6</v>
       </c>
@@ -16809,7 +16803,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
@@ -16820,7 +16814,7 @@
         <v>351.78199999999998</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="O22" s="11"/>
+      <c r="O22" s="13"/>
       <c r="P22" s="4" t="s">
         <v>7</v>
       </c>
@@ -16835,7 +16829,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="4" t="s">
         <v>8</v>
       </c>
@@ -16846,7 +16840,7 @@
         <v>532.16800000000001</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="O23" s="11"/>
+      <c r="O23" s="13"/>
       <c r="P23" s="4" t="s">
         <v>8</v>
       </c>
@@ -16908,32 +16902,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="O1" s="21" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="O1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
     </row>
     <row r="2" spans="1:19" ht="11" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
     </row>
     <row r="3" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -16964,7 +16958,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -16977,7 +16971,7 @@
         <v>0.45</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="P4" s="4" t="s">
@@ -16994,7 +16988,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -17005,7 +16999,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="O5" s="11"/>
+      <c r="O5" s="13"/>
       <c r="P5" s="4" t="s">
         <v>6</v>
       </c>
@@ -17020,7 +17014,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -17031,7 +17025,7 @@
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="O6" s="11"/>
+      <c r="O6" s="13"/>
       <c r="P6" s="4" t="s">
         <v>7</v>
       </c>
@@ -17046,7 +17040,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -17057,7 +17051,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="O7" s="11"/>
+      <c r="O7" s="13"/>
       <c r="P7" s="5" t="s">
         <v>8</v>
       </c>
@@ -17072,7 +17066,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -17085,7 +17079,7 @@
         <v>5.5119999999999996</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="O8" s="10" t="s">
+      <c r="O8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="P8" s="6" t="s">
@@ -17102,7 +17096,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -17113,7 +17107,7 @@
         <v>15.516999999999999</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="O9" s="10"/>
+      <c r="O9" s="12"/>
       <c r="P9" s="6" t="s">
         <v>6</v>
       </c>
@@ -17128,7 +17122,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
@@ -17139,7 +17133,7 @@
         <v>27.527999999999999</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="O10" s="10"/>
+      <c r="O10" s="12"/>
       <c r="P10" s="6" t="s">
         <v>7</v>
       </c>
@@ -17154,7 +17148,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
@@ -17165,7 +17159,7 @@
         <v>41.546999999999997</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="O11" s="10"/>
+      <c r="O11" s="12"/>
       <c r="P11" s="7" t="s">
         <v>8</v>
       </c>
@@ -17180,7 +17174,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -17193,7 +17187,7 @@
         <v>2.5129999999999999</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="O12" s="11" t="s">
+      <c r="O12" s="13" t="s">
         <v>10</v>
       </c>
       <c r="P12" s="4" t="s">
@@ -17210,7 +17204,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -17221,7 +17215,7 @@
         <v>3.5089999999999999</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="O13" s="11"/>
+      <c r="O13" s="13"/>
       <c r="P13" s="4" t="s">
         <v>6</v>
       </c>
@@ -17236,7 +17230,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
@@ -17247,7 +17241,7 @@
         <v>5.5090000000000003</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="O14" s="11"/>
+      <c r="O14" s="13"/>
       <c r="P14" s="4" t="s">
         <v>7</v>
       </c>
@@ -17262,7 +17256,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
@@ -17273,7 +17267,7 @@
         <v>6.5190000000000001</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="O15" s="11"/>
+      <c r="O15" s="13"/>
       <c r="P15" s="5" t="s">
         <v>8</v>
       </c>
@@ -17288,7 +17282,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -17301,7 +17295,7 @@
         <v>2.5259999999999998</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="O16" s="10" t="s">
+      <c r="O16" s="12" t="s">
         <v>11</v>
       </c>
       <c r="P16" s="6" t="s">
@@ -17318,7 +17312,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
@@ -17329,7 +17323,7 @@
         <v>5.5030000000000001</v>
       </c>
       <c r="E17" s="6"/>
-      <c r="O17" s="10"/>
+      <c r="O17" s="12"/>
       <c r="P17" s="6" t="s">
         <v>6</v>
       </c>
@@ -17344,7 +17338,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="6" t="s">
         <v>7</v>
       </c>
@@ -17355,7 +17349,7 @@
         <v>9.51</v>
       </c>
       <c r="E18" s="6"/>
-      <c r="O18" s="10"/>
+      <c r="O18" s="12"/>
       <c r="P18" s="6" t="s">
         <v>7</v>
       </c>
@@ -17370,7 +17364,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="7" t="s">
         <v>8</v>
       </c>
@@ -17381,7 +17375,7 @@
         <v>13.526</v>
       </c>
       <c r="E19" s="6"/>
-      <c r="O19" s="10"/>
+      <c r="O19" s="12"/>
       <c r="P19" s="7" t="s">
         <v>8</v>
       </c>
@@ -17396,7 +17390,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -17409,7 +17403,7 @@
         <v>44.536000000000001</v>
       </c>
       <c r="E20" s="4"/>
-      <c r="O20" s="11" t="s">
+      <c r="O20" s="13" t="s">
         <v>12</v>
       </c>
       <c r="P20" s="4" t="s">
@@ -17426,7 +17420,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
@@ -17437,7 +17431,7 @@
         <v>182.648</v>
       </c>
       <c r="E21" s="4"/>
-      <c r="O21" s="11"/>
+      <c r="O21" s="13"/>
       <c r="P21" s="4" t="s">
         <v>6</v>
       </c>
@@ -17452,7 +17446,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
@@ -17463,7 +17457,7 @@
         <v>355.83499999999998</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="O22" s="11"/>
+      <c r="O22" s="13"/>
       <c r="P22" s="4" t="s">
         <v>7</v>
       </c>
@@ -17478,7 +17472,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="4" t="s">
         <v>8</v>
       </c>
@@ -17489,7 +17483,7 @@
         <v>536.10699999999997</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="O23" s="11"/>
+      <c r="O23" s="13"/>
       <c r="P23" s="4" t="s">
         <v>8</v>
       </c>
@@ -17551,32 +17545,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="O1" s="21" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="O1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
     </row>
     <row r="3" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -17607,7 +17601,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -17620,7 +17614,7 @@
         <v>0.38600000000000001</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="P4" s="4" t="s">
@@ -17637,7 +17631,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -17648,7 +17642,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="O5" s="11"/>
+      <c r="O5" s="13"/>
       <c r="P5" s="4" t="s">
         <v>6</v>
       </c>
@@ -17663,7 +17657,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -17674,7 +17668,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="O6" s="11"/>
+      <c r="O6" s="13"/>
       <c r="P6" s="4" t="s">
         <v>7</v>
       </c>
@@ -17689,7 +17683,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -17700,7 +17694,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="O7" s="11"/>
+      <c r="O7" s="13"/>
       <c r="P7" s="5" t="s">
         <v>8</v>
       </c>
@@ -17715,7 +17709,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -17728,7 +17722,7 @@
         <v>5.49</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="O8" s="10" t="s">
+      <c r="O8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="P8" s="6" t="s">
@@ -17745,7 +17739,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -17756,7 +17750,7 @@
         <v>17.503</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="O9" s="10"/>
+      <c r="O9" s="12"/>
       <c r="P9" s="6" t="s">
         <v>6</v>
       </c>
@@ -17771,7 +17765,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
@@ -17782,7 +17776,7 @@
         <v>29.558</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="O10" s="10"/>
+      <c r="O10" s="12"/>
       <c r="P10" s="6" t="s">
         <v>7</v>
       </c>
@@ -17797,7 +17791,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
@@ -17808,7 +17802,7 @@
         <v>45.526000000000003</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="O11" s="10"/>
+      <c r="O11" s="12"/>
       <c r="P11" s="7" t="s">
         <v>8</v>
       </c>
@@ -17823,7 +17817,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -17836,7 +17830,7 @@
         <v>2.4740000000000002</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="O12" s="11" t="s">
+      <c r="O12" s="13" t="s">
         <v>10</v>
       </c>
       <c r="P12" s="4" t="s">
@@ -17853,7 +17847,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -17864,7 +17858,7 @@
         <v>3.4750000000000001</v>
       </c>
       <c r="E13" s="4"/>
-      <c r="O13" s="11"/>
+      <c r="O13" s="13"/>
       <c r="P13" s="4" t="s">
         <v>6</v>
       </c>
@@ -17879,7 +17873,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
@@ -17890,7 +17884,7 @@
         <v>6.4779999999999998</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="O14" s="11"/>
+      <c r="O14" s="13"/>
       <c r="P14" s="4" t="s">
         <v>7</v>
       </c>
@@ -17905,7 +17899,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
@@ -17916,7 +17910,7 @@
         <v>8.4930000000000003</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="O15" s="11"/>
+      <c r="O15" s="13"/>
       <c r="P15" s="5" t="s">
         <v>8</v>
       </c>
@@ -17931,7 +17925,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -17944,7 +17938,7 @@
         <v>2.4729999999999999</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="O16" s="10" t="s">
+      <c r="O16" s="12" t="s">
         <v>11</v>
       </c>
       <c r="P16" s="6" t="s">
@@ -17961,7 +17955,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
@@ -17972,7 +17966,7 @@
         <v>7.4790000000000001</v>
       </c>
       <c r="E17" s="6"/>
-      <c r="O17" s="10"/>
+      <c r="O17" s="12"/>
       <c r="P17" s="6" t="s">
         <v>6</v>
       </c>
@@ -17987,7 +17981,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="6" t="s">
         <v>7</v>
       </c>
@@ -17998,7 +17992,7 @@
         <v>10.484999999999999</v>
       </c>
       <c r="E18" s="6"/>
-      <c r="O18" s="10"/>
+      <c r="O18" s="12"/>
       <c r="P18" s="6" t="s">
         <v>7</v>
       </c>
@@ -18013,7 +18007,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="7" t="s">
         <v>8</v>
       </c>
@@ -18024,7 +18018,7 @@
         <v>15.489000000000001</v>
       </c>
       <c r="E19" s="6"/>
-      <c r="O19" s="10"/>
+      <c r="O19" s="12"/>
       <c r="P19" s="7" t="s">
         <v>8</v>
       </c>
@@ -18039,7 +18033,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -18052,7 +18046,7 @@
         <v>46.494999999999997</v>
       </c>
       <c r="E20" s="4"/>
-      <c r="O20" s="11" t="s">
+      <c r="O20" s="13" t="s">
         <v>12</v>
       </c>
       <c r="P20" s="4" t="s">
@@ -18069,7 +18063,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
@@ -18080,7 +18074,7 @@
         <v>196.59899999999999</v>
       </c>
       <c r="E21" s="4"/>
-      <c r="O21" s="11"/>
+      <c r="O21" s="13"/>
       <c r="P21" s="4" t="s">
         <v>6</v>
       </c>
@@ -18095,7 +18089,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
@@ -18106,7 +18100,7 @@
         <v>379.82900000000001</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="O22" s="11"/>
+      <c r="O22" s="13"/>
       <c r="P22" s="4" t="s">
         <v>7</v>
       </c>
@@ -18121,7 +18115,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="4" t="s">
         <v>8</v>
       </c>
@@ -18132,7 +18126,7 @@
         <v>570.06100000000004</v>
       </c>
       <c r="E23" s="4"/>
-      <c r="O23" s="11"/>
+      <c r="O23" s="13"/>
       <c r="P23" s="4" t="s">
         <v>8</v>
       </c>
@@ -18196,32 +18190,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="70" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="O1" s="21" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="O1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
     </row>
     <row r="2" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
     </row>
     <row r="3" spans="1:19" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -18252,7 +18246,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -18282,7 +18276,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -18308,7 +18302,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -18334,7 +18328,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -18360,7 +18354,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -18373,7 +18367,7 @@
         <v>5.5259999999999998</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="O8" s="14" t="s">
+      <c r="O8" s="20" t="s">
         <v>9</v>
       </c>
       <c r="P8" s="6" t="s">
@@ -18390,7 +18384,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -18401,7 +18395,7 @@
         <v>16.507000000000001</v>
       </c>
       <c r="E9" s="6"/>
-      <c r="O9" s="15"/>
+      <c r="O9" s="21"/>
       <c r="P9" s="6" t="s">
         <v>6</v>
       </c>
@@ -18416,7 +18410,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
@@ -18427,7 +18421,7 @@
         <v>30.51</v>
       </c>
       <c r="E10" s="6"/>
-      <c r="O10" s="15"/>
+      <c r="O10" s="21"/>
       <c r="P10" s="6" t="s">
         <v>7</v>
       </c>
@@ -18442,7 +18436,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
@@ -18453,7 +18447,7 @@
         <v>44.54</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="O11" s="16"/>
+      <c r="O11" s="22"/>
       <c r="P11" s="7" t="s">
         <v>8</v>
       </c>
@@ -18468,7 +18462,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -18498,7 +18492,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -18524,7 +18518,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
@@ -18550,7 +18544,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
@@ -18576,7 +18570,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -18589,7 +18583,7 @@
         <v>3.4990000000000001</v>
       </c>
       <c r="E16" s="6"/>
-      <c r="O16" s="14" t="s">
+      <c r="O16" s="20" t="s">
         <v>11</v>
       </c>
       <c r="P16" s="6" t="s">
@@ -18606,7 +18600,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
@@ -18617,7 +18611,7 @@
         <v>7.4950000000000001</v>
       </c>
       <c r="E17" s="6"/>
-      <c r="O17" s="15"/>
+      <c r="O17" s="21"/>
       <c r="P17" s="6" t="s">
         <v>6</v>
       </c>
@@ -18632,7 +18626,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="6" t="s">
         <v>7</v>
       </c>
@@ -18643,7 +18637,7 @@
         <v>11.51</v>
       </c>
       <c r="E18" s="6"/>
-      <c r="O18" s="15"/>
+      <c r="O18" s="21"/>
       <c r="P18" s="6" t="s">
         <v>7</v>
       </c>
@@ -18658,7 +18652,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="7" t="s">
         <v>8</v>
       </c>
@@ -18669,7 +18663,7 @@
         <v>15.510999999999999</v>
       </c>
       <c r="E19" s="6"/>
-      <c r="O19" s="16"/>
+      <c r="O19" s="22"/>
       <c r="P19" s="7" t="s">
         <v>8</v>
       </c>
@@ -18684,7 +18678,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -18714,7 +18708,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
@@ -18740,7 +18734,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
@@ -18766,7 +18760,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" ht="19" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="4" t="s">
         <v>8</v>
       </c>
@@ -18818,7 +18812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -18846,32 +18840,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="61" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="O1" s="21" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="O1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
     </row>
     <row r="2" spans="1:19" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
     </row>
     <row r="3" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -18902,7 +18896,7 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -18917,7 +18911,7 @@
       <c r="E4" s="4">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="P4" s="4" t="s">
@@ -18934,7 +18928,7 @@
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
@@ -18947,7 +18941,7 @@
       <c r="E5" s="4">
         <v>1.8979999999999999</v>
       </c>
-      <c r="O5" s="11"/>
+      <c r="O5" s="13"/>
       <c r="P5" s="4" t="s">
         <v>6</v>
       </c>
@@ -18962,7 +18956,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
@@ -18975,7 +18969,7 @@
       <c r="E6" s="4">
         <v>2.23</v>
       </c>
-      <c r="O6" s="11"/>
+      <c r="O6" s="13"/>
       <c r="P6" s="4" t="s">
         <v>7</v>
       </c>
@@ -18990,7 +18984,7 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -19003,7 +18997,7 @@
       <c r="E7" s="4">
         <v>0.115</v>
       </c>
-      <c r="O7" s="11"/>
+      <c r="O7" s="13"/>
       <c r="P7" s="5" t="s">
         <v>8</v>
       </c>
@@ -19018,7 +19012,7 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -19033,7 +19027,7 @@
       <c r="E8" s="6">
         <v>6.4690000000000003</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="O8" s="12" t="s">
         <v>9</v>
       </c>
       <c r="P8" s="6" t="s">
@@ -19050,7 +19044,7 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
@@ -19063,7 +19057,7 @@
       <c r="E9" s="6">
         <v>21.295999999999999</v>
       </c>
-      <c r="O9" s="10"/>
+      <c r="O9" s="12"/>
       <c r="P9" s="6" t="s">
         <v>6</v>
       </c>
@@ -19078,7 +19072,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
@@ -19091,7 +19085,7 @@
       <c r="E10" s="6">
         <v>42.765999999999998</v>
       </c>
-      <c r="O10" s="10"/>
+      <c r="O10" s="12"/>
       <c r="P10" s="6" t="s">
         <v>7</v>
       </c>
@@ -19106,7 +19100,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
@@ -19119,7 +19113,7 @@
       <c r="E11" s="6">
         <v>56.95</v>
       </c>
-      <c r="O11" s="10"/>
+      <c r="O11" s="12"/>
       <c r="P11" s="7" t="s">
         <v>8</v>
       </c>
@@ -19134,7 +19128,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -19149,7 +19143,7 @@
       <c r="E12" s="4">
         <v>2.4830000000000001</v>
       </c>
-      <c r="O12" s="11" t="s">
+      <c r="O12" s="13" t="s">
         <v>10</v>
       </c>
       <c r="P12" s="4" t="s">
@@ -19166,7 +19160,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
@@ -19179,7 +19173,7 @@
       <c r="E13" s="4">
         <v>6.6180000000000003</v>
       </c>
-      <c r="O13" s="11"/>
+      <c r="O13" s="13"/>
       <c r="P13" s="4" t="s">
         <v>6</v>
       </c>
@@ -19194,7 +19188,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
@@ -19207,7 +19201,7 @@
       <c r="E14" s="4">
         <v>10.647</v>
       </c>
-      <c r="O14" s="11"/>
+      <c r="O14" s="13"/>
       <c r="P14" s="4" t="s">
         <v>7</v>
       </c>
@@ -19222,7 +19216,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
@@ -19235,7 +19229,7 @@
       <c r="E15" s="4">
         <v>16.623999999999999</v>
       </c>
-      <c r="O15" s="11"/>
+      <c r="O15" s="13"/>
       <c r="P15" s="5" t="s">
         <v>8</v>
       </c>
@@ -19250,7 +19244,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -19265,7 +19259,7 @@
       <c r="E16" s="6">
         <v>4.4690000000000003</v>
       </c>
-      <c r="O16" s="10" t="s">
+      <c r="O16" s="12" t="s">
         <v>11</v>
       </c>
       <c r="P16" s="6" t="s">
@@ -19282,7 +19276,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
@@ -19295,7 +19289,7 @@
       <c r="E17" s="6">
         <v>11.548999999999999</v>
       </c>
-      <c r="O17" s="10"/>
+      <c r="O17" s="12"/>
       <c r="P17" s="6" t="s">
         <v>6</v>
       </c>
@@ -19310,7 +19304,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="12"/>
       <c r="B18" s="6" t="s">
         <v>7</v>
       </c>
@@ -19323,7 +19317,7 @@
       <c r="E18" s="6">
         <v>24.692</v>
       </c>
-      <c r="O18" s="10"/>
+      <c r="O18" s="12"/>
       <c r="P18" s="6" t="s">
         <v>7</v>
       </c>
@@ -19338,7 +19332,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="7" t="s">
         <v>8</v>
       </c>
@@ -19351,7 +19345,7 @@
       <c r="E19" s="6">
         <v>36.997</v>
       </c>
-      <c r="O19" s="10"/>
+      <c r="O19" s="12"/>
       <c r="P19" s="7" t="s">
         <v>8</v>
       </c>
@@ -19366,7 +19360,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -19381,7 +19375,7 @@
       <c r="E20" s="4">
         <v>329.65100000000001</v>
       </c>
-      <c r="O20" s="11" t="s">
+      <c r="O20" s="13" t="s">
         <v>12</v>
       </c>
       <c r="P20" s="4" t="s">
@@ -19398,7 +19392,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
@@ -19411,7 +19405,7 @@
       <c r="E21" s="4">
         <v>1337.89</v>
       </c>
-      <c r="O21" s="11"/>
+      <c r="O21" s="13"/>
       <c r="P21" s="4" t="s">
         <v>6</v>
       </c>
@@ -19426,7 +19420,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
+      <c r="A22" s="13"/>
       <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
@@ -19439,7 +19433,7 @@
       <c r="E22" s="4">
         <v>2616.904</v>
       </c>
-      <c r="O22" s="11"/>
+      <c r="O22" s="13"/>
       <c r="P22" s="4" t="s">
         <v>7</v>
       </c>
@@ -19454,7 +19448,7 @@
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="4" t="s">
         <v>8</v>
       </c>
@@ -19467,7 +19461,7 @@
       <c r="E23" s="4">
         <v>3990.2330000000002</v>
       </c>
-      <c r="O23" s="11"/>
+      <c r="O23" s="13"/>
       <c r="P23" s="4" t="s">
         <v>8</v>
       </c>

</xml_diff>